<commit_message>
add  SR6009_IR_BJ project for nbiot-beijing water meter
</commit_message>
<xml_diff>
--- a/doc/A380产品型号&软件描述.xlsx
+++ b/doc/A380产品型号&软件描述.xlsx
@@ -72,10 +72,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>用于6009A抄表(和龙定制)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>用于8009抄表(濮阳定制)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -250,6 +246,10 @@
       </rPr>
       <t>X</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用于6009抄表(和龙定制)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -693,7 +693,7 @@
   <dimension ref="B3:F20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -711,7 +711,7 @@
     </row>
     <row r="5" spans="2:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>0</v>
@@ -720,15 +720,15 @@
         <v>1</v>
       </c>
       <c r="E5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>16</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>2</v>
@@ -737,15 +737,15 @@
         <v>3</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>6</v>
@@ -754,10 +754,10 @@
         <v>9</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -769,7 +769,7 @@
     </row>
     <row r="9" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>4</v>
@@ -778,10 +778,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -793,7 +793,7 @@
     </row>
     <row r="11" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>7</v>
@@ -802,15 +802,15 @@
         <v>10</v>
       </c>
       <c r="E11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>8</v>
@@ -819,10 +819,10 @@
         <v>11</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -834,20 +834,20 @@
     </row>
     <row r="14" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>7</v>
@@ -867,13 +867,13 @@
     </row>
     <row r="17" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>

</xml_diff>